<commit_message>
2024AA releasedoc moving folder structure
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F5B4070-4B0D-443F-A927-2BF25371A596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF702830-A212-4946-9002-6987685640CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
+    <workbookView xWindow="10692" yWindow="48" windowWidth="12312" windowHeight="12144" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
   </bookViews>
   <sheets>
     <sheet name="2024AA" sheetId="1" r:id="rId1"/>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -655,19 +655,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1068,7 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="19" t="s">
         <v>148</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -1086,7 +1079,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
@@ -1113,7 +1106,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
@@ -1128,14 +1121,14 @@
       <c r="F4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="18" t="s">
         <v>142</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B5"/>
@@ -1163,7 +1156,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B6"/>
@@ -1191,7 +1184,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B7" t="s">
@@ -1219,7 +1212,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B8"/>
@@ -1247,7 +1240,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>139</v>
       </c>
       <c r="C9" t="s">
@@ -1274,7 +1267,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
@@ -1292,7 +1285,7 @@
       <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="19" t="s">
         <v>144</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -1301,7 +1294,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C11" t="s">
@@ -1326,7 +1319,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B12"/>
@@ -1355,7 +1348,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B13"/>
@@ -1381,7 +1374,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B14"/>
@@ -1407,7 +1400,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B15"/>
@@ -1433,7 +1426,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B16"/>
@@ -1450,7 +1443,7 @@
         <v>22</v>
       </c>
       <c r="G16"/>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="19" t="s">
         <v>145</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -1458,8 +1451,8 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B17"/>
@@ -1476,7 +1469,7 @@
         <v>22</v>
       </c>
       <c r="G17"/>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="19" t="s">
         <v>146</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -1484,8 +1477,8 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
@@ -1500,7 +1493,7 @@
       <c r="F18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="19" t="s">
         <v>147</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -1508,8 +1501,8 @@
       </c>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
@@ -1530,8 +1523,8 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B20"/>
@@ -1554,8 +1547,8 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B21"/>
@@ -1574,7 +1567,7 @@
       <c r="G21" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="19" t="s">
         <v>143</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -1582,8 +1575,8 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B22"/>
@@ -1608,8 +1601,8 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B23"/>
@@ -1634,24 +1627,24 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24"/>
+      <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="13">
         <v>12</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="3"/>
@@ -1660,34 +1653,33 @@
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21" t="s">
+      <c r="B25"/>
+      <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="13">
         <v>12</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="K25" s="21"/>
-    </row>
-    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="H25"/>
+      <c r="I25" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
@@ -1703,12 +1695,11 @@
       <c r="G26" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="21"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="C27" t="s">
@@ -1727,7 +1718,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
2024AA updates and checks on remaining release documentation files
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF702830-A212-4946-9002-6987685640CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE56ABC-9CD5-440B-8C67-18B99C31ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10692" yWindow="48" windowWidth="12312" windowHeight="12144" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
   </bookViews>
   <sheets>
     <sheet name="2024AA" sheetId="1" r:id="rId1"/>
     <sheet name="2024AA sources count" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024AA'!$A$1:$J$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024AA'!$A$1:$L$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="149">
   <si>
     <t>Name of page</t>
   </si>
@@ -477,16 +477,16 @@
     <t>Update with text from TB article</t>
   </si>
   <si>
-    <t>Check these</t>
-  </si>
-  <si>
-    <t>Update</t>
-  </si>
-  <si>
-    <t>Check this</t>
-  </si>
-  <si>
     <t>In teamsite make sure each file has the most updated version</t>
+  </si>
+  <si>
+    <t>https://www.nlm.nih.gov/research/umls/index.html</t>
+  </si>
+  <si>
+    <t>Publish on release day</t>
+  </si>
+  <si>
+    <t>Teamsite umls/</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,8 +560,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -570,11 +576,22 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -582,30 +599,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -614,11 +618,22 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -628,7 +643,79 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -637,30 +724,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,737 +1106,795 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="18.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="27.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="37" style="4" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="18.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="9"/>
+    <col min="7" max="7" width="27.21875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="10" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="8.88671875" style="3"/>
+    <col min="13" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="42"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="43"/>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10">
+        <v>12</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10">
+        <v>12</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10">
+        <v>11</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="43"/>
+      <c r="K7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10">
+        <v>11</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="44"/>
+      <c r="K8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="28">
+        <v>1</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="10">
+        <v>3</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="10">
+        <v>6</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="10">
+        <v>8</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="10">
+        <v>12</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:12" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10">
+        <v>12</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="10">
+        <v>12</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="31"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="10">
+        <v>12</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="10">
+        <v>12</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="10">
+        <v>13</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="10">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="G22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="10">
+        <v>5</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="10">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="13">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="G24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K24" s="21"/>
+    </row>
+    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="10">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="13">
-        <v>2</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="G25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="10">
         <v>6</v>
       </c>
-      <c r="B6"/>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="13">
-        <v>2</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="13">
-        <v>3</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="G26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="41"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="10">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="13">
-        <v>4</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="13">
-        <v>5</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="13">
-        <v>6</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="13">
-        <v>6</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="13">
-        <v>7</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13"/>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="13">
-        <v>8</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14"/>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="13">
-        <v>9</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15"/>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="13">
-        <v>10</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16"/>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="13">
-        <v>11</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16"/>
-      <c r="H16" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17"/>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="13">
-        <v>11</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17"/>
-      <c r="H17" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="13">
-        <v>11</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="13">
-        <v>12</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20"/>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="13">
-        <v>12</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21"/>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="13">
-        <v>12</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22"/>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="13">
-        <v>12</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23"/>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="13">
-        <v>12</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24"/>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="13">
-        <v>12</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25"/>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="13">
-        <v>12</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25"/>
-      <c r="I25" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="H27" s="3"/>
+      <c r="I27" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J27" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J27">
+  <autoFilter ref="A1:L27" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L27">
       <sortCondition ref="E1:E27"/>
     </sortState>
   </autoFilter>
@@ -1748,22 +1917,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H4" t="s">
@@ -1771,7 +1940,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H5" t="s">
@@ -1779,7 +1948,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H6" t="s">
@@ -1787,367 +1956,367 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="2" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2024AA updates to release doc archive files
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE56ABC-9CD5-440B-8C67-18B99C31ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14DE46C-A7CD-41F4-BD70-5D89E06A87DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="2024AA sources count" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024AA'!$A$1:$L$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024AA'!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="153">
   <si>
     <t>Name of page</t>
   </si>
@@ -462,9 +462,6 @@
     <t>version_Release Notes and Bugs_final</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>https://wiki.nlm.nih.gov/confluence/display/UMLS/UMLS+release+documentation+procedures</t>
   </si>
   <si>
@@ -487,6 +484,21 @@
   </si>
   <si>
     <t>Teamsite umls/</t>
+  </si>
+  <si>
+    <t>Saved in Teamsite, just need to hit submit</t>
+  </si>
+  <si>
+    <t>https://www.nlm.nih.gov/research/umls/archive/archive_home.html</t>
+  </si>
+  <si>
+    <t>Make table widths equal</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>https://www.nlm.nih.gov/research/umls/licensedcontent/umlsarchives04.html</t>
   </si>
 </sst>
 </file>
@@ -535,7 +547,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,12 +568,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -609,7 +615,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -621,7 +667,42 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -629,93 +710,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -724,54 +726,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,796 +1104,833 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" style="4" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="4"/>
-    <col min="5" max="5" width="18.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="9"/>
-    <col min="7" max="7" width="27.21875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="4"/>
-    <col min="10" max="10" width="10" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="37" style="3" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="11.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="23.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="10" style="3" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="3"/>
-    <col min="13" max="16384" width="8.88671875" style="4"/>
+    <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="L1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="39"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="28"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="24"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="24"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="24"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="28"/>
+      <c r="K14" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B15" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H15" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="K15" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="28"/>
+      <c r="K19" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="23"/>
+      <c r="M19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="34"/>
+      <c r="I20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="28"/>
+      <c r="K20" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="25"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="27"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="23"/>
+    </row>
+    <row r="25" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="27"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="23"/>
+    </row>
+    <row r="26" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="I26" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="27"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="23"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="10">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="G27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="H27" s="38"/>
+      <c r="I27" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="35"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="37"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="10">
-        <v>12</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="10">
-        <v>11</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="43"/>
-      <c r="K7" s="22"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="10">
-        <v>11</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="44"/>
-      <c r="K8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="10">
-        <v>11</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="28">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="10">
-        <v>2</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="10">
-        <v>2</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="10">
-        <v>3</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="10">
-        <v>6</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="10">
-        <v>8</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="10">
-        <v>12</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="10">
-        <v>12</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="10">
-        <v>12</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="31"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="10">
-        <v>12</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="10">
-        <v>12</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="24"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="10">
-        <v>13</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="24"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="10">
-        <v>4</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="10">
-        <v>5</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="10">
-        <v>9</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K24" s="21"/>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="10">
-        <v>10</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K25" s="21"/>
-    </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="10">
-        <v>6</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="41"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="10">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="26"/>
-      <c r="K27" s="27"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>141</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L27" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L27">
-      <sortCondition ref="E1:E27"/>
+  <autoFilter ref="A1:M27" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M27">
+      <sortCondition descending="1" ref="G1:G27"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2024AA release docs checklist update
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14DE46C-A7CD-41F4-BD70-5D89E06A87DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E4615B-FD30-49DB-B9E2-CB8071C5206B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
+    <workbookView xWindow="10692" yWindow="48" windowWidth="12312" windowHeight="12144" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
   </bookViews>
   <sheets>
     <sheet name="2024AA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
   <si>
     <t>Name of page</t>
   </si>
@@ -726,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -737,16 +737,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -756,20 +750,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,13 +1140,13 @@
       <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="14" t="s">
         <v>50</v>
       </c>
       <c r="L1" s="7" t="s">
@@ -1167,7 +1157,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B2"/>
@@ -1186,15 +1176,15 @@
       <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" t="s">
         <v>148</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="40"/>
+      <c r="I2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="28"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1217,12 +1207,12 @@
         <v>26</v>
       </c>
       <c r="H3"/>
-      <c r="I3" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="24"/>
+      <c r="I3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1245,12 +1235,12 @@
         <v>26</v>
       </c>
       <c r="H4"/>
-      <c r="I4" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="24"/>
+      <c r="I4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1275,12 +1265,12 @@
         <v>26</v>
       </c>
       <c r="H5"/>
-      <c r="I5" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="24"/>
+      <c r="I5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1305,12 +1295,12 @@
       <c r="H6" t="s">
         <v>143</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="24"/>
+      <c r="I6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1335,12 +1325,12 @@
       <c r="H7" t="s">
         <v>142</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="24"/>
+      <c r="I7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1359,16 +1349,16 @@
       <c r="F8">
         <v>12</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="24"/>
+      <c r="H8"/>
+      <c r="I8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1389,12 +1379,12 @@
       <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="24"/>
+      <c r="I9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1415,12 +1405,12 @@
       <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="24"/>
+      <c r="I10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1441,12 +1431,12 @@
       <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="24"/>
+      <c r="I11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1469,15 +1459,15 @@
         <v>26</v>
       </c>
       <c r="H12"/>
-      <c r="I12" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="24"/>
+      <c r="I12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="21"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
       <c r="B13"/>
@@ -1496,18 +1486,18 @@
       <c r="G13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="18"/>
+      <c r="H13"/>
+      <c r="I13" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C14" t="s">
@@ -1525,21 +1515,21 @@
       <c r="G14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="28"/>
-      <c r="K14" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="23"/>
+      <c r="H14"/>
+      <c r="I14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="17"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" t="s">
         <v>149</v>
       </c>
       <c r="C15" t="s">
@@ -1557,17 +1547,17 @@
       <c r="G15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" t="s">
         <v>144</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L15" s="25"/>
+      <c r="I15" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="19"/>
       <c r="M15" t="s">
         <v>55</v>
       </c>
@@ -1591,15 +1581,14 @@
       <c r="G16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="28"/>
-      <c r="K16" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="25"/>
+      <c r="I16" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1620,15 +1609,14 @@
       <c r="G17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L17" s="17"/>
+      <c r="I17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1647,24 +1635,24 @@
       <c r="F18">
         <v>2</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="25"/>
+      <c r="H18"/>
+      <c r="I18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="21"/>
+      <c r="K18" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" t="s">
         <v>152</v>
       </c>
       <c r="C19" t="s">
@@ -1682,17 +1670,17 @@
       <c r="G19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="23"/>
+      <c r="I19" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="17"/>
       <c r="M19" t="s">
         <v>150</v>
       </c>
@@ -1716,18 +1704,18 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="I20" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L20" s="25"/>
+      <c r="H20"/>
+      <c r="I20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1749,12 +1737,14 @@
         <v>22</v>
       </c>
       <c r="H21"/>
-      <c r="I21" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="27"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="18"/>
+      <c r="I21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="12"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1777,12 +1767,14 @@
         <v>22</v>
       </c>
       <c r="H22"/>
-      <c r="I22" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="18"/>
+      <c r="I22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="12"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1805,12 +1797,14 @@
         <v>22</v>
       </c>
       <c r="H23"/>
-      <c r="I23" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="27"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="23"/>
+      <c r="I23" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="17"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1833,12 +1827,14 @@
         <v>22</v>
       </c>
       <c r="H24"/>
-      <c r="I24" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="23"/>
+      <c r="I24" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="23"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1859,13 +1855,14 @@
       <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="27"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="23"/>
+      <c r="I25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="17"/>
     </row>
     <row r="26" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1887,12 +1884,14 @@
         <v>22</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="27"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="23"/>
+      <c r="I26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="23"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1914,13 +1913,14 @@
       <c r="G27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="38"/>
-      <c r="I27" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="35"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="37"/>
+      <c r="I27" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">

</xml_diff>

<commit_message>
2024AA release day docs checklist
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/Checklist for release docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E4615B-FD30-49DB-B9E2-CB8071C5206B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79A246D-8F0D-4C0F-AF19-C9DCE1FD7D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10692" yWindow="48" windowWidth="12312" windowHeight="12144" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783A2471-F8C4-4A9E-8256-38911F8C9201}"/>
   </bookViews>
   <sheets>
     <sheet name="2024AA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="157">
   <si>
     <t>Name of page</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Public page</t>
   </si>
   <si>
-    <t>When it should be published</t>
-  </si>
-  <si>
     <t>Type of file</t>
   </si>
   <si>
@@ -499,13 +496,28 @@
   </si>
   <si>
     <t>https://www.nlm.nih.gov/research/umls/licensedcontent/umlsarchives04.html</t>
+  </si>
+  <si>
+    <t>Change script so it excludes the back to top target blank</t>
+  </si>
+  <si>
+    <t>Need to update the format to bold and bullet points</t>
+  </si>
+  <si>
+    <t>https://uts.nlm.nih.gov/uts/assets/LicenseAgreement.pdf</t>
+  </si>
+  <si>
+    <t>When it should be completed</t>
+  </si>
+  <si>
+    <t>https://uts.nlm.nih.gov/uts/assets/licenseText.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,8 +558,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,8 +595,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -624,30 +653,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -668,17 +677,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -726,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -741,25 +739,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8B074E-C582-4CF3-9203-F5D6ABC65115}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,808 +1120,843 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="L1" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>37</v>
+      <c r="A2" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="29"/>
+        <v>147</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>43</v>
+      <c r="A3" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3"/>
-      <c r="I3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="18"/>
+      <c r="I3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
+      <c r="A4" s="28" t="s">
+        <v>43</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4"/>
-      <c r="I4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="18"/>
+      <c r="I4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
+      <c r="A5" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5"/>
-      <c r="I5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="18"/>
+      <c r="I5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>34</v>
+      <c r="A6" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="18"/>
+        <v>142</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>29</v>
+      <c r="A7" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>142</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="18"/>
+        <v>141</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>30</v>
+      <c r="A8" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8"/>
-      <c r="I8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="18"/>
+      <c r="I8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>31</v>
+      <c r="A9" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>32</v>
+      <c r="A10" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>33</v>
+      <c r="A11" s="28" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
+      <c r="A12" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>13</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12"/>
-      <c r="I12" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="18"/>
+      <c r="I12" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13"/>
-      <c r="I13" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="12"/>
+      <c r="I13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="K13" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>11</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14"/>
-      <c r="I14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="17"/>
+      <c r="I14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>144</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L15" s="19"/>
+        <v>143</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="K15" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="25"/>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="19"/>
+        <v>38</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="J17" s="11"/>
-      <c r="K17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L17" s="11"/>
+      <c r="K17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18"/>
-      <c r="I18" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="19"/>
+      <c r="I18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="20"/>
       <c r="M19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20"/>
-      <c r="I20" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L20" s="19"/>
+      <c r="I20" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <v>12</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21"/>
-      <c r="I21" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="12"/>
+      <c r="I21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>154</v>
+      </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22">
         <v>12</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22"/>
-      <c r="I22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="12"/>
+      <c r="I22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23"/>
-      <c r="I23" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="23"/>
-      <c r="L23" s="17"/>
+      <c r="I23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="19"/>
+      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24">
         <v>5</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24"/>
-      <c r="I24" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="23"/>
-      <c r="L24" s="17"/>
+      <c r="I24" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="19"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>46</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25">
         <v>6</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="F26">
         <v>9</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" s="23"/>
-      <c r="L26" s="17"/>
+      <c r="I26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27"/>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="F27">
         <v>10</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
+        <v>21</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="22"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1953,406 +1985,406 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>